<commit_message>
finished dataImporter's function to import troop and castle data, where properly input,  from an associated workbook, and insert the parsed data into the database
</commit_message>
<xml_diff>
--- a/SandboxServer/src/main/resources/data.xlsx
+++ b/SandboxServer/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Castle" sheetId="1" r:id="rId1"/>
@@ -20,33 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
-  <si>
-    <t>1A</t>
-  </si>
-  <si>
-    <t>1B</t>
-  </si>
-  <si>
-    <t>1C</t>
-  </si>
-  <si>
-    <t>2A</t>
-  </si>
-  <si>
-    <t>2B</t>
-  </si>
-  <si>
-    <t>2C</t>
-  </si>
-  <si>
-    <t>3A</t>
-  </si>
-  <si>
-    <t>3B</t>
-  </si>
-  <si>
-    <t>3C</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Troop Name</t>
+  </si>
+  <si>
+    <t>Salute</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Yes sir?</t>
+  </si>
+  <si>
+    <t>Yes sir!</t>
+  </si>
+  <si>
+    <t>Talison</t>
+  </si>
+  <si>
+    <t>Castle Name</t>
+  </si>
+  <si>
+    <t>Faction</t>
+  </si>
+  <si>
+    <t>Wall Strength</t>
+  </si>
+  <si>
+    <t>Castle at Old Town</t>
+  </si>
+  <si>
+    <t>Knights of the Round</t>
+  </si>
+  <si>
+    <t>Troops</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -364,45 +382,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>20000</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -412,15 +439,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A10075-568F-4087-BBFC-5519A636092C}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,27 +463,30 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>